<commit_message>
adding the final test for the argument reference experiment
</commit_message>
<xml_diff>
--- a/CVS Files/Ads prompt/01.08.22/annotation/GOLD vs Clusters.xlsx
+++ b/CVS Files/Ads prompt/01.08.22/annotation/GOLD vs Clusters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USERS-Load\PycharmProjects\pythonProject\CVS Files\01.08.22\annotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USERS-Load\PycharmProjects\pythonProject\CVS Files\Ads prompt\01.08.22\annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0478E6A7-D0E7-4C4A-A22F-E6E7AE2FF03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A86C72-651B-41EC-AA08-D473BB9C27E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,7 +455,7 @@
     <t>purity =  70.73170731707317</t>
   </si>
   <si>
-    <t>Auto calculated using cosin similarity for 5 items of each cluster</t>
+    <t>Auto calculated using manually assessted data for 5 items of each cluster</t>
   </si>
 </sst>
 </file>
@@ -865,7 +865,7 @@
   <dimension ref="A1:AA83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A2:C9"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,7 +873,7 @@
     <col min="2" max="2" width="141.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="60.21875" customWidth="1"/>
+    <col min="7" max="7" width="143.33203125" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>